<commit_message>
[v1.0.8] - added public api documents - updateExpress.js   - update database based on separate xlsx file - updateSuburb_test.js   - test script to prevent from exhausting  all API call counts
</commit_message>
<xml_diff>
--- a/scripts/test.xlsx
+++ b/scripts/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cadenzah/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FB7816F-0315-1C43-96F6-A643BD4B1FE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C340B603-258D-8743-9BD1-347D8D5E5665}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="300" yWindow="460" windowWidth="25000" windowHeight="15000" xr2:uid="{F487CCE0-92A7-EE4C-8ADA-F04DB4F7A9EE}"/>
   </bookViews>
@@ -30,9 +30,50 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+  <si>
+    <t>NAEK176</t>
+  </si>
+  <si>
+    <t>안중오거리</t>
+  </si>
+  <si>
+    <t>평택시</t>
+  </si>
+  <si>
+    <t>NAEK177</t>
+  </si>
+  <si>
+    <t>안중</t>
+  </si>
+  <si>
+    <t>NAEK339</t>
+  </si>
+  <si>
+    <t>아산온양</t>
+  </si>
+  <si>
+    <t>아산시</t>
+  </si>
+  <si>
+    <t>locationName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cityCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>locationCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -43,6 +84,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
@@ -71,8 +120,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -389,12 +441,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{950D7136-27F3-1E44-BB91-5AC4197D4702}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>31070</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>31070</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1">
+        <v>34040</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>